<commit_message>
initial ipsc implementation, fixes for diff cell import
</commit_message>
<xml_diff>
--- a/sampledata/sample_differentiated_cell_batches.xlsx
+++ b/sampledata/sample_differentiated_cell_batches.xlsx
@@ -78,7 +78,7 @@
     <t>Most Recent Update</t>
   </si>
   <si>
-    <t>HMSL70001</t>
+    <t>HMSL75001</t>
   </si>
   <si>
     <t>center_name1</t>
@@ -141,7 +141,7 @@
     <t>transient modification 2</t>
   </si>
   <si>
-    <t>HMSL70002</t>
+    <t>HMSL75002</t>
   </si>
   <si>
     <t>center_name2a</t>
@@ -189,7 +189,7 @@
     <t>transient modification 4</t>
   </si>
   <si>
-    <t>HMSL70003</t>
+    <t>HMSL75003</t>
   </si>
   <si>
     <t>center_name3c</t>
@@ -234,7 +234,7 @@
     <t>transient modification 6</t>
   </si>
   <si>
-    <t>HMSL70004</t>
+    <t>HMSL75004</t>
   </si>
   <si>
     <t>center_name7</t>
@@ -270,7 +270,7 @@
     <t>transient modification 8</t>
   </si>
   <si>
-    <t>HMSL70005</t>
+    <t>HMSL75005</t>
   </si>
   <si>
     <t>center_name9</t>
@@ -291,7 +291,7 @@
     <t>transient modification 9</t>
   </si>
   <si>
-    <t>HMSL70006</t>
+    <t>HMSL75006</t>
   </si>
   <si>
     <t>center_name10</t>
@@ -312,7 +312,7 @@
     <t>transient modification 10</t>
   </si>
   <si>
-    <t>HMSL70007</t>
+    <t>HMSL75007</t>
   </si>
   <si>
     <t>center_name11</t>
@@ -330,7 +330,7 @@
     <t>transient modification 11</t>
   </si>
   <si>
-    <t>HMSL70008</t>
+    <t>HMSL75008</t>
   </si>
   <si>
     <t>center_name12</t>
@@ -348,7 +348,7 @@
     <t>transient modification 12</t>
   </si>
   <si>
-    <t>HMSL70009</t>
+    <t>HMSL75009</t>
   </si>
   <si>
     <t>center_name13</t>
@@ -562,26 +562,27 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,7 +1097,7 @@
         <v>88</v>
       </c>
       <c r="B12" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>89</v>
@@ -1327,7 +1328,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="9" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="9" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
hide the Center_Specific_Code from detail/list views
</commit_message>
<xml_diff>
--- a/sampledata/sample_differentiated_cell_batches.xlsx
+++ b/sampledata/sample_differentiated_cell_batches.xlsx
@@ -81,7 +81,7 @@
     <t>HMSL75001</t>
   </si>
   <si>
-    <t>center_name1</t>
+    <t>hms batch name 1</t>
   </si>
   <si>
     <t>ATCC</t>
@@ -117,7 +117,7 @@
     <t>2015-05-23</t>
   </si>
   <si>
-    <t>center_name1a</t>
+    <t>hms batch name 1a</t>
   </si>
   <si>
     <t>ECACC</t>
@@ -144,7 +144,7 @@
     <t>HMSL75002</t>
   </si>
   <si>
-    <t>center_name2a</t>
+    <t>hms batch name2a</t>
   </si>
   <si>
     <t>DSMZ</t>
@@ -168,7 +168,7 @@
     <t>2015-06-01</t>
   </si>
   <si>
-    <t>center_name2</t>
+    <t>hms batch name2</t>
   </si>
   <si>
     <t>HTB-103a</t>
@@ -192,7 +192,7 @@
     <t>HMSL75003</t>
   </si>
   <si>
-    <t>center_name3c</t>
+    <t>hms batch name3c</t>
   </si>
   <si>
     <t>CRL-1872</t>
@@ -213,7 +213,7 @@
     <t>transient modification 5</t>
   </si>
   <si>
-    <t>center_name3-3</t>
+    <t>hms batch name3-3</t>
   </si>
   <si>
     <t>CRL-1739</t>
@@ -237,7 +237,7 @@
     <t>HMSL75004</t>
   </si>
   <si>
-    <t>center_name7</t>
+    <t>hms batch name7</t>
   </si>
   <si>
     <t>ACC 143</t>
@@ -273,7 +273,7 @@
     <t>HMSL75005</t>
   </si>
   <si>
-    <t>center_name9</t>
+    <t>hms batch name9</t>
   </si>
   <si>
     <t>JHSF</t>
@@ -294,7 +294,7 @@
     <t>HMSL75006</t>
   </si>
   <si>
-    <t>center_name10</t>
+    <t>hms batch name10</t>
   </si>
   <si>
     <t>ACC 302</t>
@@ -315,7 +315,7 @@
     <t>HMSL75007</t>
   </si>
   <si>
-    <t>center_name11</t>
+    <t>hms batch name11</t>
   </si>
   <si>
     <t>HTB-54</t>
@@ -333,7 +333,7 @@
     <t>HMSL75008</t>
   </si>
   <si>
-    <t>center_name12</t>
+    <t>hms batch name12</t>
   </si>
   <si>
     <t>HTB-55</t>
@@ -351,7 +351,7 @@
     <t>HMSL75009</t>
   </si>
   <si>
-    <t>center_name13</t>
+    <t>hms batch name13</t>
   </si>
   <si>
     <t>ACC 264</t>
@@ -566,23 +566,23 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="C5" activeCellId="0" sqref="C5:C9 C11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,12 +1323,12 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C5:C9 C11:C15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="9" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="9" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>